<commit_message>
adjusted pivot table on nav ratio
</commit_message>
<xml_diff>
--- a/Survey of pilot - sept 2013.xlsx
+++ b/Survey of pilot - sept 2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="-15" windowWidth="25905" windowHeight="13440"/>
+    <workbookView xWindow="1875" yWindow="-15" windowWidth="10620" windowHeight="8715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>Q1. How would you rate your knowledge of structured navigation commands prior to using the blaze tool?</t>
   </si>
@@ -114,9 +115,6 @@
     <t>while double clicking blaze info, VS is restarting</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>vs</t>
   </si>
   <si>
@@ -159,9 +157,6 @@
     <t>will blaze work with multiple instances</t>
   </si>
   <si>
-    <t>7 out of 10</t>
-  </si>
-  <si>
     <t>not at all</t>
   </si>
   <si>
@@ -183,9 +178,6 @@
     <t>mohan</t>
   </si>
   <si>
-    <t>90% usage</t>
-  </si>
-  <si>
     <t>sando</t>
   </si>
   <si>
@@ -249,16 +241,64 @@
     <t>Points</t>
   </si>
   <si>
-    <t>Navigation Ratio Average</t>
-  </si>
-  <si>
     <t>Days of blaze usage</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Average Navigtion Ratio</t>
+  </si>
+  <si>
+    <t>Navigation Ratio</t>
+  </si>
+  <si>
+    <t>Week1</t>
+  </si>
+  <si>
+    <t>Week2</t>
+  </si>
+  <si>
+    <t>Week3</t>
+  </si>
+  <si>
+    <t>Week4</t>
+  </si>
+  <si>
+    <t>Week5</t>
+  </si>
+  <si>
+    <t>I work in code I wrote</t>
+  </si>
+  <si>
+    <t>I recently learned code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -296,13 +336,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,12 +646,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="675" topLeftCell="A10" activePane="bottomLeft"/>
+      <pane ySplit="675" topLeftCell="A22" activePane="bottomLeft"/>
       <selection activeCell="C33" sqref="C33"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,679 +662,881 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
+      <c r="B3" s="3">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
         <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
         <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
       <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" t="s">
-        <v>16</v>
-      </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="G19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23">
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
         <v>8</v>
       </c>
-      <c r="D23">
-        <v>9</v>
-      </c>
-      <c r="E23">
+      <c r="C26">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
         <v>7</v>
       </c>
-      <c r="F23">
-        <v>6</v>
-      </c>
-      <c r="G23">
+      <c r="F26">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
+      <c r="G26">
         <v>8</v>
       </c>
-      <c r="C25">
-        <v>14</v>
-      </c>
-      <c r="D25">
-        <v>10</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>7</v>
-      </c>
-      <c r="G25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>27</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>26</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>26</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35">
+        <v>432</v>
+      </c>
+      <c r="C35">
+        <v>78</v>
+      </c>
+      <c r="D35">
+        <v>464</v>
+      </c>
+      <c r="E35">
+        <v>101</v>
+      </c>
+      <c r="F35">
+        <v>84</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>42</v>
+      </c>
+      <c r="E36">
+        <v>38</v>
+      </c>
+      <c r="F36">
+        <v>38</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="J36" s="4">
+        <f>AVERAGE(E38:G38,B38)</f>
+        <v>1.7546389958504077E-2</v>
+      </c>
+      <c r="K36" s="4">
+        <f>AVERAGE(C38:D38)</f>
+        <v>2.7673352300158799E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="4">
+        <v>8.0009328354031101E-3</v>
+      </c>
+      <c r="C38" s="4">
+        <v>3.5003673333965306E-2</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2.0343031266352288E-2</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3.344907390333049E-2</v>
+      </c>
+      <c r="F38" s="4">
+        <v>2.7802717274387181E-2</v>
+      </c>
+      <c r="G38" s="4">
+        <v>9.3283582089552237E-4</v>
+      </c>
+      <c r="I38">
+        <v>2.0338779570018398E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" t="s">
         <v>76</v>
       </c>
-      <c r="B34">
-        <v>432</v>
-      </c>
-      <c r="C34">
+      <c r="G40" t="s">
         <v>78</v>
       </c>
-      <c r="D34">
-        <v>464</v>
-      </c>
-      <c r="E34">
-        <v>101</v>
-      </c>
-      <c r="F34">
+      <c r="I40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35">
-        <v>32</v>
-      </c>
-      <c r="C35">
-        <v>14</v>
-      </c>
-      <c r="D35">
-        <v>42</v>
-      </c>
-      <c r="E35">
-        <v>38</v>
-      </c>
-      <c r="F35">
-        <v>38</v>
-      </c>
-      <c r="G35">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36">
-        <v>8.0009328354031101E-3</v>
-      </c>
-      <c r="C36">
-        <v>2.1897810218978103E-2</v>
-      </c>
-      <c r="D36">
-        <v>2.0076452869346055E-2</v>
-      </c>
-      <c r="E36">
-        <v>3.0408249003027719E-2</v>
-      </c>
-      <c r="F36" t="e">
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>2.9459901800327332E-2</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1.8790100824931256E-2</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2.0253164556962026E-2</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G41" s="4">
+        <v>1.9267822736030828E-3</v>
+      </c>
+      <c r="I41">
+        <v>1.643835616438356E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="4">
+        <v>6.8587105624142658E-3</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1.1650485436893204E-2</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2.1739130434782608E-2</v>
+      </c>
+      <c r="E42" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="G36">
-        <v>9.3283582089552237E-4</v>
-      </c>
+      <c r="F42" s="4">
+        <v>4.1935483870967745E-2</v>
+      </c>
+      <c r="G42" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1.6615895873719193E-2</v>
+      </c>
+      <c r="C43" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D43" s="4">
+        <v>4.9638989169675093E-3</v>
+      </c>
+      <c r="E43" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="4">
+        <v>4.1361158112427146E-3</v>
+      </c>
+      <c r="C44" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1.0471204188481676E-2</v>
+      </c>
+      <c r="E44" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F44" s="4">
+        <v>4.1067761806981518E-2</v>
+      </c>
+      <c r="G44" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44">
+        <v>1.673469387755102E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="4">
+        <v>3.2617559119325905E-3</v>
+      </c>
+      <c r="C45" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1.5275707898658718E-2</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.6525198938992044E-2</v>
+      </c>
+      <c r="F45" s="4">
+        <v>4.1128084606345476E-2</v>
+      </c>
+      <c r="G45" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45">
+        <v>7.1105365223012281E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:K4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:K5">
       <formula1>"As much as possible, many times, some, not much, not at all"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:K5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:K6">
       <formula1>"All new to me,  Several items were new to me, A few were new to me, Nothing was new to me, I did not review the info"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:K6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:K7">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:K7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:K8">
       <formula1>"Very helpful, somewhat helpful, neither helpful nor unhelpful, not helpful, I did not use it"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:K10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:K11">
       <formula1>"A lot, some, a little, not at all"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:K18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:K19">
       <formula1>"Testing and debugging, Locating the source of a bug, Designing a bug fix implementation, Designing a new feature implementation, Implementing a bug fix, Implementing a new feature, Refactoring"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:K20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:K21">
       <formula1>"Much more, more, about the same, less, much less"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:K23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:K24">
       <formula1>"0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26:K26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27:K27">
       <formula1>"I work in code that I wrote, I work in code that I did not author but maintain regularly, I recently learned the code I work in, I work in code I am not familiar with"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1313,7 +1556,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1321,7 +1564,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1329,7 +1572,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1337,7 +1580,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1345,9 +1588,9 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="3">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2">
         <f>B1/B4-B2/B4</f>
         <v>-0.33333333333333337</v>
       </c>

</xml_diff>